<commit_message>
some changes not important
</commit_message>
<xml_diff>
--- a/macro_factor/indicators/inputs/otr_bond10y.xlsx
+++ b/macro_factor/indicators/inputs/otr_bond10y.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>100019.IB</t>
   </si>
@@ -131,6 +131,10 @@
   </si>
   <si>
     <t>200006.IB</t>
+  </si>
+  <si>
+    <t>200016.IB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -497,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A39"/>
+  <dimension ref="A1:A40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -703,6 +707,11 @@
         <v>38</v>
       </c>
     </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>